<commit_message>
Updated the config file on MaxRetryNumber to 2 in preparation for transaction processing. Added the initial extract communication list sequence.
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\eFinance\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCFB91C-39F7-4100-A961-B7EDB1A13E4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977E832A-BBAF-4B43-9B3C-261A8569C031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -524,15 +524,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="113.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="113.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -581,7 +581,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1620,14 +1620,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1664,12 +1666,12 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
@@ -2732,12 +2734,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Created an \Output folder
Added entries to the gitignore file. Will ignore now the created Excel file as part of debugging. Will ignore as well any future files created in the \Output folder
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\eFinance\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B297EF-4C7C-40D3-96A7-1388B0697C19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2438E611-5D3B-454A-BFAD-4EF8FEDC6E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="444" windowWidth="22200" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>eFinanceCommunicationApprovalProcess</t>
+  </si>
+  <si>
+    <t>Download_Directory</t>
+  </si>
+  <si>
+    <t>\Output</t>
+  </si>
+  <si>
+    <t>Directory to where the attachments will be downloaded and processed</t>
   </si>
 </sst>
 </file>
@@ -511,15 +520,15 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="113.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="113.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -556,7 +565,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -589,7 +598,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1598,12 +1617,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1640,7 +1659,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2708,12 +2727,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Config.xlsx: Added the ProcessedData_File entry
Main.xaml : Added in the initialization the building of 2 data table (dt_SuccessData and dt_ExceptionData) which will contain the processed data information and its status.
Also added as input / output arguments in the success and exception data table when invoking the SetTransactionStatus workflow
Lastly, added the sequence for generating the processed data report.

SetTransactionStatus.xaml : Added the addition io arguments for the success and exception data table. Added the add data row activity for the success data in the success flow. Added the add data row activity for the exception data in the business exception flow.

PRocess.xaml - added an activity to throw a business exception whenever data being processed contains a blank username.
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2438E611-5D3B-454A-BFAD-4EF8FEDC6E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E76628-8299-4F43-B7BB-AE25F2630784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Directory to where the attachments will be downloaded and processed</t>
+  </si>
+  <si>
+    <t>\Output\ProcessedData.xlsx</t>
+  </si>
+  <si>
+    <t>ProcessedData_File</t>
+  </si>
+  <si>
+    <t>Path and filename of excel file that will contain the list of processed data and its status.</t>
   </si>
 </sst>
 </file>
@@ -520,15 +529,15 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="113.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="113.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -565,7 +574,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -609,7 +618,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1617,12 +1636,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1659,7 +1678,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2727,12 +2746,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated the BillingStatement sequence Created the GetAttachmentsSequence
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E76628-8299-4F43-B7BB-AE25F2630784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB9BB3-4B5F-4C2F-A0B9-4E4E24D2973C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,33 @@
   </si>
   <si>
     <t>Path and filename of excel file that will contain the list of processed data and its status.</t>
+  </si>
+  <si>
+    <t>TimeoutShort</t>
+  </si>
+  <si>
+    <t>TimeoutMedium</t>
+  </si>
+  <si>
+    <t>TimeoutLong</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for activities which are likely to fail. Must be integer</t>
+  </si>
+  <si>
+    <t>Timeout medium value in milliseconds. Must be integer</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
+  </si>
+  <si>
+    <t>SupportedFileFormats</t>
+  </si>
+  <si>
+    <t>{".pdf",".jpg",".jpeg"}</t>
+  </si>
+  <si>
+    <t>List of all supported file formats for the GetAttachments.xaml workflow</t>
   </si>
 </sst>
 </file>
@@ -529,15 +556,15 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="113.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="113.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -574,7 +601,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -629,7 +656,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1633,15 +1670,15 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1678,7 +1715,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1758,9 +1795,39 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>5000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>30000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>120000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2746,12 +2813,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Linked GetAttachmentsSquence and DownloadFiles xaml
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnfe.NNITCORP\Documents\UiPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB9BB3-4B5F-4C2F-A0B9-4E4E24D2973C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D34496-16ED-4FAE-9263-C687998D4648}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -166,10 +166,10 @@
     <t>SupportedFileFormats</t>
   </si>
   <si>
-    <t>{".pdf",".jpg",".jpeg"}</t>
-  </si>
-  <si>
     <t>List of all supported file formats for the GetAttachments.xaml workflow</t>
+  </si>
+  <si>
+    <t>{".pdf",".jpg",".jpeg",".png"}</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -661,10 +661,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Placeholder for Cutoff limit New XAML Config additional row
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2438E611-5D3B-454A-BFAD-4EF8FEDC6E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -134,12 +133,18 @@
   </si>
   <si>
     <t>Directory to where the attachments will be downloaded and processed</t>
+  </si>
+  <si>
+    <t>Cutoff</t>
+  </si>
+  <si>
+    <t>Cut off limit of records to be processed. Only records before the set cutoff should be processed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -151,6 +156,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -169,6 +175,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -202,6 +209,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,11 +524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -609,7 +617,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1601,8 +1616,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{0CBB09DF-41D1-4243-95B0-32554F851625}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{1A0B967A-88F1-4633-B7AD-B3CEED0ADE20}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1610,7 +1625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2722,7 +2737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
updated config to reflect cutoff
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnfe.NNITCORP\Documents\UiPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath2\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D34496-16ED-4FAE-9263-C687998D4648}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -170,12 +169,18 @@
   </si>
   <si>
     <t>{".pdf",".jpg",".jpeg",".png"}</t>
+  </si>
+  <si>
+    <t>CutOff</t>
+  </si>
+  <si>
+    <t>This is where the cutoff date is set, only those submitted reimbursement on or before the set cutoff will be processed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -187,6 +192,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -205,6 +211,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -238,6 +245,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -552,11 +560,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -667,7 +675,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1657,8 +1672,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{0CBB09DF-41D1-4243-95B0-32554F851625}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{1A0B967A-88F1-4633-B7AD-B3CEED0ADE20}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1666,7 +1681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2808,7 +2823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated Cutoff limit flow to handle updating value in config file
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath2\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -246,6 +246,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,6 +679,9 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>49</v>
+      </c>
+      <c r="B8" s="6">
+        <v>44028</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Renamed GetAttachmentsSequence and added functionality to extract the bill number from the entry. Further integrated sequences to the Main.xaml. Updated various sequences part of REFramework.
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90786EDE-3C63-4907-8CD7-71107CDEB20F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -180,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -561,11 +562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1676,8 +1677,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1685,7 +1686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2827,7 +2828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated the logic of most flows
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90786EDE-3C63-4907-8CD7-71107CDEB20F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD67CBE-C7D5-4FA9-B237-D059ED493D3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,13 +169,13 @@
     <t>List of all supported file formats for the GetAttachments.xaml workflow</t>
   </si>
   <si>
-    <t>{".pdf",".jpg",".jpeg",".png"}</t>
-  </si>
-  <si>
     <t>CutOff</t>
   </si>
   <si>
     <t>This is where the cutoff date is set, only those submitted reimbursement on or before the set cutoff will be processed</t>
+  </si>
+  <si>
+    <t>.pdf, .jpg, .jpeg, .png</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6">
         <v>44028</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added a while loop in the Get_Attachment... sequence in order for it to accommodate large files being downloaded. Adjusted Click to click on the top left corner for reliability Edited the ProcessedData_File entry value in the Config file
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD67CBE-C7D5-4FA9-B237-D059ED493D3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A723D0C-2984-4DE8-B2D9-C952622F2F41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>Download_Directory</t>
   </si>
   <si>
-    <t>\Output</t>
-  </si>
-  <si>
     <t>Directory to where the attachments will be downloaded and processed</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>.pdf, .jpg, .jpeg, .png</t>
+  </si>
+  <si>
+    <t>\Downloads</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -649,43 +649,43 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6">
         <v>44028</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1817,35 +1817,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>5000</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>30000</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>120000</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Enhanced the reliability of the DownloadPdf sequence. Added Downloads folder to separate the contents of the Output folder
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A723D0C-2984-4DE8-B2D9-C952622F2F41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535F206E-F66A-4B7D-8593-B63335A1C718}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,9 +133,6 @@
     <t>Directory to where the attachments will be downloaded and processed</t>
   </si>
   <si>
-    <t>\Output\ProcessedData.xlsx</t>
-  </si>
-  <si>
     <t>ProcessedData_File</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>\Downloads</t>
+  </si>
+  <si>
+    <t>Output\ProcessedData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -649,7 +649,7 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -657,35 +657,35 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6">
         <v>44028</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1817,35 +1817,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>5000</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>30000</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>120000</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated to point to preprod site
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath_Integrated\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535F206E-F66A-4B7D-8593-B63335A1C718}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC16DE-8B46-4114-B12E-267FC18B6A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -109,15 +109,9 @@
     <t>CommAllItems</t>
   </si>
   <si>
-    <t>http://workit.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/AllItems.aspx</t>
-  </si>
-  <si>
     <t>Comm_EntryPage</t>
   </si>
   <si>
-    <t>http://workit.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/DispForm.aspx?ID=</t>
-  </si>
-  <si>
     <t>Webpage. Contains all the communication reimbursements filed by every employee</t>
   </si>
   <si>
@@ -176,6 +170,12 @@
   </si>
   <si>
     <t>Output\ProcessedData.xlsx</t>
+  </si>
+  <si>
+    <t>http://workitpreprod.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/2019.aspx</t>
+  </si>
+  <si>
+    <t>http://workitpreprod.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/DispForm.aspx?ID=</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -616,7 +616,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
@@ -627,65 +627,65 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="6">
         <v>44028</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1817,35 +1817,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>5000</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>30000</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>120000</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added small handling like 'Continue on errors'.
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath_Appid\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603F0DD3-5318-4ACD-A9DF-97654A55129A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3885" yWindow="4140" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -123,9 +124,6 @@
     <t>Download_Directory</t>
   </si>
   <si>
-    <t>\Output</t>
-  </si>
-  <si>
     <t>Directory to where the attachments will be downloaded and processed</t>
   </si>
   <si>
@@ -163,12 +161,6 @@
   </si>
   <si>
     <t>{".pdf",".jpg",".jpeg",".png"}</t>
-  </si>
-  <si>
-    <t>http://workitpreprod.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/2020.aspx</t>
-  </si>
-  <si>
-    <t>http://workitpreprod.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/DispForm.aspx?ID=</t>
   </si>
   <si>
     <t>CutOff</t>
@@ -179,12 +171,21 @@
   <si>
     <t xml:space="preserve">This is where the cutoff date is set, only those submitted reimbursement on or before the set cutoff will be processed
 </t>
+  </si>
+  <si>
+    <t>http://workit.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/AllItems.aspx</t>
+  </si>
+  <si>
+    <t>http://workit.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/DispForm.aspx?ID=</t>
+  </si>
+  <si>
+    <t>\Downloads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -564,11 +565,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -629,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -640,7 +641,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -651,43 +652,43 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1678,20 +1679,16 @@
     <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1819,35 +1816,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>5000</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>30000</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>120000</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2830,7 +2827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added OR, Month, Amount paid columns on the output excel Updated config to point to preprod environment
</commit_message>
<xml_diff>
--- a/eFinance_Process/Data/Config.xlsx
+++ b/eFinance_Process/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVV\Downloads\Plans\UIPath\eFinancePH_UIPath\eFinance_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdjc\Documents\UiPath\POC\eFinancePH_UIPath\eFinance_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603F0DD3-5318-4ACD-A9DF-97654A55129A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE689E38-CAED-4428-A78B-1DB01317B193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="4140" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -173,13 +173,13 @@
 </t>
   </si>
   <si>
-    <t>http://workit.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/AllItems.aspx</t>
-  </si>
-  <si>
-    <t>http://workit.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/DispForm.aspx?ID=</t>
-  </si>
-  <si>
     <t>\Downloads</t>
+  </si>
+  <si>
+    <t>http://workitpreprod.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/2020.aspx</t>
+  </si>
+  <si>
+    <t>http://workitpreprod.nnitcorp.com/Departments/399-1000/Corporate/Finance/e-Finance/Lists/Communication/DispForm.aspx?ID=</t>
   </si>
 </sst>
 </file>
@@ -568,16 +568,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="113.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="113.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -614,7 +614,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -630,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -641,7 +641,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -652,7 +652,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -1679,8 +1679,12 @@
     <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{D4BA7E4A-C49B-4CFB-BB4C-B5FD86960AD2}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{55B81F0D-7154-4866-ABE8-6E12E9A14DE0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1688,16 +1692,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1734,7 +1738,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2832,12 +2836,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>